<commit_message>
Updated src and documents folder
</commit_message>
<xml_diff>
--- a/documents/Published/TreemapBarChart/TreemapBarChartByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/TreemapBarChart/TreemapBarChartByMAQSoftwareChecklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub_CustomVisuals\documents\Published\TreemapBarChart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual\documents\Published\TreemapBarChart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F625D7-8FBE-45F5-A42B-7287E8A53C36}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055C840B-9220-4B1E-806A-AD0C8EB36DA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{15650058-D9E1-4E2D-A421-D272244BB495}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="115">
   <si>
     <r>
       <t>#</t>
@@ -445,6 +445,24 @@
     <t>1. Go to formatting pane
 2. Go to 'Legend'. Update the position to 'Top-Centre'
 3.Update the Text-size to 14                                                                          4.Update the Legend color to 'Red'</t>
+  </si>
+  <si>
+    <t>PowerBi</t>
+  </si>
+  <si>
+    <t>Internet expl</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>edge</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Same</t>
   </si>
 </sst>
 </file>
@@ -633,6 +651,2123 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>28047</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1410325</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1448469</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB2DED3F-C313-4BFE-8FFA-3644E14BB726}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14144625" y="409047"/>
+          <a:ext cx="1324600" cy="1420422"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>204079</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1676400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1445694</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D9322FC-2CF7-4325-9AD0-28E6C27C060C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15796504" y="390524"/>
+          <a:ext cx="1472321" cy="1436170"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>92748</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1486390</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1445348</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69B81E47-0D72-4E7D-8538-8695A7FE06F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19716750" y="473748"/>
+          <a:ext cx="1286365" cy="1352600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>17005</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1543631</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1464958</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4AA9D9C-B749-49E8-A3B2-13BEBEA180A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17821274" y="398005"/>
+          <a:ext cx="1381707" cy="1447953"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>49396</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1648446</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1638952</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{822CBAA7-3FB8-4DF6-BD59-E2BBC9B6F91E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14192250" y="1906771"/>
+          <a:ext cx="1515096" cy="1589556"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>78351</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1857952</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1743661</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30165A08-A79D-429C-A19C-44A5C4A9A58E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16325850" y="1935726"/>
+          <a:ext cx="1638877" cy="1665310"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1771650</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1478227</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01979E78-129E-43ED-8E19-5F18B432C4EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18240375" y="2171700"/>
+          <a:ext cx="1704975" cy="1163902"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>182245</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1466849</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1553845</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36CBB0B2-2C49-4E96-8802-8246395F27D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20212049" y="2039620"/>
+          <a:ext cx="1285875" cy="1371600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>209993</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1648449</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1658007</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C951652-CECF-482B-9B12-544A8C7C5751}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14268893" y="3790950"/>
+          <a:ext cx="1438456" cy="1515132"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>305828</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>276225</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1896105</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1638841</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDB1985F-A14D-4FA0-A0C5-C1C8990319DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16412603" y="3924300"/>
+          <a:ext cx="1590277" cy="1362616"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>79629</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1781428</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1647825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88AAB321-15C5-49A7-96FC-B162EFDDF0E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18253329" y="3733800"/>
+          <a:ext cx="1701799" cy="1562100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>175427</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1448285</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1534041</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE5B0EF6-E928-4133-B0A4-085EA94EACEC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20206502" y="3829050"/>
+          <a:ext cx="1272858" cy="1353066"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>72527</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2540892</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1666875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C67526DD-55CB-4E58-87DD-F85D68BDC82A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18246227" y="5857874"/>
+          <a:ext cx="2468365" cy="1609726"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>142653</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1753229</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1505495</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D4FD8FC-EF68-4131-B3AF-8AB6FB926563}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16287750" y="5943378"/>
+          <a:ext cx="1572254" cy="1362842"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>34707</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1914525</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1810500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64E7396B-B22F-4BC7-892F-16A6CC53714F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14116049" y="5835432"/>
+          <a:ext cx="1857376" cy="1775793"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>89057</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1800707</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1772170</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6945675-E83A-49ED-B952-C19739C2A386}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21078824" y="5889782"/>
+          <a:ext cx="1562583" cy="1683113"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>107576</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2524125</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1419224</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{938BC673-4CD5-49FD-890C-9C951ACBE5CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18281276" y="7753349"/>
+          <a:ext cx="2416549" cy="1304925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>171449</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>60270</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1943724</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1591214</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56BB866C-CD0A-4F11-9B61-A4E444BD886A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16278224" y="7699320"/>
+          <a:ext cx="1772275" cy="1530944"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>50148</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1724516</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1638816</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDFA5A44-9F14-4A0B-A66C-66FC2FDFEF3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21050249" y="7689198"/>
+          <a:ext cx="1514967" cy="1588668"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>30879</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1715121</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1629437</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FA53B9B-FE44-4EA8-B900-822445B42D0A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14277975" y="7669929"/>
+          <a:ext cx="1496046" cy="1598558"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>94961</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1685924</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1742263</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CE34BF9-54CE-4A11-BB7B-E6D6DB969743}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14153861" y="9363074"/>
+          <a:ext cx="1590963" cy="1675589"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>153859</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1867525</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1562637</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95225A27-0903-48F2-8BB9-85574C6CCDB8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16335375" y="9450259"/>
+          <a:ext cx="1638925" cy="1408778"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>80756</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2571751</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1638911</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE06AC07-6725-4AE3-964F-9E3BE50A2646}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18211801" y="9377156"/>
+          <a:ext cx="2533650" cy="1558155"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>62191</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1962149</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1745208</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7E5AF0E-1E21-4840-8573-40F0419BAC5A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20907374" y="9358591"/>
+          <a:ext cx="1895475" cy="1683017"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1714788</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1704164</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2E8E2E9-AA7B-4EF2-9D5D-5E288F4C4A4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14182725" y="11153775"/>
+          <a:ext cx="1590963" cy="1675589"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1772275</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1523078</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A8DB842-12B9-4CB9-BBAB-A9D8D68C3DBA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16240125" y="11239500"/>
+          <a:ext cx="1638925" cy="1408778"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2600325</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1643880</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3993A71A-44AD-4021-83C3-36440F455B5F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18240375" y="11210925"/>
+          <a:ext cx="2533650" cy="1558155"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1981200</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1749692</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{159EB73B-1FAF-4252-B559-C9FD11BE4F38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20926425" y="11191875"/>
+          <a:ext cx="1895475" cy="1683017"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>114301</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1771651</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1817894</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{320167FA-A45E-4485-AFD2-84EAF755CC35}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14173201" y="13087350"/>
+          <a:ext cx="1657350" cy="1675019"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>67986</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2048500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1886490</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5D9FA92-8F85-4B5C-A553-35FAC5BA68B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16174761" y="13115924"/>
+          <a:ext cx="1980514" cy="1715041"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>268361</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2496594</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1591263</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Picture 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFC02281-9FE6-47A1-AA06-1F1A9901FF4C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18326100" y="13212836"/>
+          <a:ext cx="2344194" cy="1322902"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>59910</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1923189</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1952625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Picture 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7CD0337-C7C7-4FDD-BD68-77F490D04E2D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20907374" y="13004385"/>
+          <a:ext cx="1856515" cy="1892715"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>190499</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>179774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2000702</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1676775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="Picture 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{539BECA9-2C2A-4C5D-B4B0-881A1926A6DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14249399" y="15153074"/>
+          <a:ext cx="1810203" cy="1497001"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1996247</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1619251</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="Picture 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47362292-75BC-4E36-B943-62B3983CEEF7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16163925" y="15068551"/>
+          <a:ext cx="1939097" cy="1524000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>44742</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2209799</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1669569</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="Picture 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42D6E93E-A437-441C-92E2-DF382044DAF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18468974" y="15018042"/>
+          <a:ext cx="1914525" cy="1624827"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>87072</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1991120</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1619576</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Picture 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7B5346D-F1A1-4376-8DCB-7C41D41B932F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20974050" y="15060372"/>
+          <a:ext cx="1857770" cy="1532504"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>47624</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>32868</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1924050</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1455760</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="42" name="Picture 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0921C24E-3F41-40C3-81EE-015FD2C493CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14106524" y="17273118"/>
+          <a:ext cx="1876426" cy="1422892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>138436</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1972437</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1438808</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="Picture 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8262F34A-FF81-481A-A63E-6C7DD3E521D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16221075" y="17378686"/>
+          <a:ext cx="1858137" cy="1300372"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>55911</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2655987</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1333500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="44" name="Picture 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE61BAA8-75DB-46D1-BAEA-D0E04DDE0E6C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18240375" y="17296161"/>
+          <a:ext cx="2589312" cy="1277589"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>51207</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1515076</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1400779</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Picture 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A20AF049-D566-44BA-AE8E-51E4993CF257}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21012150" y="17291457"/>
+          <a:ext cx="1343626" cy="1349572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>47624</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1924050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1715722</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="50" name="Picture 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F4AC2BD-3C6F-4FCC-8F28-4B9B6D37F02C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14106524" y="21599525"/>
+          <a:ext cx="1876426" cy="1652222"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>224659</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1794313</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1771650</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="51" name="Picture 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07526509-BC89-439F-A2D1-5DD6D7FFAE26}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16331434" y="21621750"/>
+          <a:ext cx="1569654" cy="1685925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>13790</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2619375</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1810353</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="52" name="Picture 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3746E4C2-E64F-41B5-969A-97CC64718232}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18259425" y="21549815"/>
+          <a:ext cx="2533650" cy="1796563"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>67388</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>41274</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1866900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="53" name="Picture 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD255600-1470-42CC-A901-0650AF9418A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20916900" y="19507913"/>
+          <a:ext cx="2289174" cy="1799512"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>45823</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2219789</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1791102</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="54" name="Picture 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A9F1E4A-C07C-4F1A-A423-F6494DE311D8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18383250" y="19486348"/>
+          <a:ext cx="2010239" cy="1745279"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>138911</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1978670</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1847851</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="55" name="Picture 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F0E0CB8-E02E-46C2-8E10-D8AC3DA58A3A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16259174" y="19579436"/>
+          <a:ext cx="1826271" cy="1708940"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>209551</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2009775</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1758135</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="56" name="Picture 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97E007D1-11FB-4729-B98E-F4725AA572BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14220825" y="19650076"/>
+          <a:ext cx="1847850" cy="1548584"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>333376</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>108144</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1999750</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1857376</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="57" name="Picture 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95F4DD84-AA3B-42E2-AAEB-98284DD4C785}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21174076" y="21644169"/>
+          <a:ext cx="1666374" cy="1749232"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -934,8 +3069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AD304B0-4792-43AB-9D20-CD62C2AB01B6}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,7 +3079,10 @@
     <col min="3" max="3" width="47" customWidth="1"/>
     <col min="4" max="4" width="56.5703125" customWidth="1"/>
     <col min="5" max="5" width="55.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="7" max="7" width="31" customWidth="1"/>
+    <col min="8" max="8" width="40" customWidth="1"/>
+    <col min="9" max="9" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -969,12 +3107,20 @@
       <c r="E2" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-    </row>
-    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="F2" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -995,7 +3141,7 @@
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="141" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>2</v>
       </c>
@@ -1016,7 +3162,7 @@
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>3</v>
       </c>
@@ -1053,12 +3199,20 @@
       <c r="E6" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-    </row>
-    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="F6" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>5</v>
       </c>
@@ -1079,7 +3233,7 @@
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
     </row>
-    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>6</v>
       </c>
@@ -1100,7 +3254,7 @@
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
     </row>
-    <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="144" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>7</v>
       </c>
@@ -1121,7 +3275,7 @@
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
     </row>
-    <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>8</v>
       </c>
@@ -1142,7 +3296,7 @@
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>9</v>
       </c>
@@ -1163,7 +3317,7 @@
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>10</v>
       </c>
@@ -1184,7 +3338,7 @@
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
     </row>
-    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>11</v>
       </c>
@@ -1200,12 +3354,20 @@
       <c r="E13" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-    </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="F13" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>12</v>
       </c>
@@ -1242,8 +3404,20 @@
       <c r="E15" s="10" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="F15" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>14</v>
       </c>
@@ -1259,8 +3433,20 @@
       <c r="E16" s="10" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="F16" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="165" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>15</v>
       </c>
@@ -1277,7 +3463,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>16</v>
       </c>
@@ -1300,6 +3486,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>